<commit_message>
More of Statistics for DA
</commit_message>
<xml_diff>
--- a/Statistics for Data Science and Business Analysis/Section 3/2.4.Numerical-variables.Frequency-distribution-table-exercise.xlsx
+++ b/Statistics for Data Science and Business Analysis/Section 3/2.4.Numerical-variables.Frequency-distribution-table-exercise.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iliya\Desktop\Statistics Course\Filming\Final excel\Section 2 - Descriptive statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cursos de Mi Repositorio\Statistics for Data Science and Business Analysis\Section 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281DDF45-6CDE-4F48-8E56-FEE0DAEC2908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequency distribution table" sheetId="10" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Numerical variables. Frequency distribution table</t>
   </si>
@@ -64,13 +73,40 @@
   </si>
   <si>
     <t>Given that we want to divide the numbers into 6 intervals of equal width, calculate that interval width. Round up to the nearest whole number, bigger than the result that you obtain</t>
+  </si>
+  <si>
+    <t>Desired intervals</t>
+  </si>
+  <si>
+    <t>Interval width</t>
+  </si>
+  <si>
+    <t>Interval start</t>
+  </si>
+  <si>
+    <t>Interval end</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Relative frequency</t>
+  </si>
+  <si>
+    <t>2 - Frequency distribution table</t>
+  </si>
+  <si>
+    <t>3 - Frequency distribution table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +161,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -140,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -157,11 +200,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF002060"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -205,8 +267,54 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -223,7 +331,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -518,36 +626,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="19" width="8.88671875" style="3"/>
-    <col min="20" max="20" width="10.44140625" style="3" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="19" width="8.85546875" style="3"/>
+    <col min="20" max="20" width="10.42578125" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
@@ -555,7 +665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
@@ -563,7 +673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
@@ -586,7 +696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
@@ -601,9 +711,12 @@
     <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>1</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="Q12" s="1"/>
     </row>
@@ -611,17 +724,32 @@
       <c r="B13" s="3">
         <v>8</v>
       </c>
+      <c r="D13" s="5"/>
       <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>30</v>
       </c>
+      <c r="D14" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="21">
+        <v>6</v>
+      </c>
+      <c r="F14" s="22"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="2:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>30</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="21">
+        <f>ROUNDUP((B32-B13)/E14,0)</f>
+        <v>46</v>
       </c>
       <c r="I15" s="8"/>
       <c r="Q15" s="2"/>
@@ -630,16 +758,25 @@
       <c r="B16" s="3">
         <v>50</v>
       </c>
+      <c r="D16" s="5"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="2:17" ht="13.2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>86</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="H17" s="11"/>
       <c r="I17" s="10"/>
       <c r="J17" s="11"/>
@@ -654,10 +791,21 @@
       <c r="B18" s="3">
         <v>94</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="D18" s="23">
+        <v>8</v>
+      </c>
+      <c r="E18" s="23">
+        <f>D18+E15</f>
+        <v>54</v>
+      </c>
+      <c r="F18" s="23">
+        <f>COUNTIFS($B$13:$B$32,"&gt;="&amp;D18,$B$13:$B$32,"&lt;="&amp;E18)</f>
+        <v>4</v>
+      </c>
+      <c r="G18" s="24">
+        <f>F18/COUNT($B$13:$B$32)</f>
+        <v>0.2</v>
+      </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -668,15 +816,27 @@
       <c r="O18" s="9"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="2:17" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>102</v>
       </c>
       <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="11"/>
+      <c r="D19" s="23">
+        <f>E18</f>
+        <v>54</v>
+      </c>
+      <c r="E19" s="23">
+        <f>D19+E15</f>
+        <v>100</v>
+      </c>
+      <c r="F19" s="23">
+        <f t="shared" ref="F19:F23" si="0">COUNTIFS($B$13:$B$32,"&gt;="&amp;D19,$B$13:$B$32,"&lt;="&amp;E19)</f>
+        <v>2</v>
+      </c>
+      <c r="G19" s="24">
+        <f t="shared" ref="G19:G24" si="1">F19/COUNT($B$13:$B$32)</f>
+        <v>0.1</v>
+      </c>
       <c r="H19" s="11"/>
       <c r="I19" s="7"/>
       <c r="J19" s="12"/>
@@ -686,15 +846,27 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
-    <row r="20" spans="2:17" ht="12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>110</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="D20" s="23">
+        <f>E19</f>
+        <v>100</v>
+      </c>
+      <c r="E20" s="23">
+        <f>D20+E15</f>
+        <v>146</v>
+      </c>
+      <c r="F20" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G20" s="24">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
       <c r="H20" s="11"/>
       <c r="I20" s="7"/>
       <c r="J20" s="14"/>
@@ -709,10 +881,22 @@
         <v>169</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="D21" s="23">
+        <f>E20</f>
+        <v>146</v>
+      </c>
+      <c r="E21" s="23">
+        <f>D21+E15</f>
+        <v>192</v>
+      </c>
+      <c r="F21" s="23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G21" s="24">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -722,15 +906,27 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" spans="2:17" ht="12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>170</v>
       </c>
       <c r="C22" s="9"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
+      <c r="D22" s="23">
+        <f>E21</f>
+        <v>192</v>
+      </c>
+      <c r="E22" s="23">
+        <f>D22+E15</f>
+        <v>238</v>
+      </c>
+      <c r="F22" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G22" s="24">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
       <c r="H22" s="11"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -745,10 +941,22 @@
         <v>176</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="17"/>
+      <c r="D23" s="25">
+        <f>E22</f>
+        <v>238</v>
+      </c>
+      <c r="E23" s="25">
+        <f>D23+E15</f>
+        <v>284</v>
+      </c>
+      <c r="F23" s="32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G23" s="33">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
       <c r="H23" s="11"/>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
@@ -763,10 +971,14 @@
         <v>236</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="17"/>
+      <c r="F24" s="23">
+        <f>SUM(F18:F23)</f>
+        <v>20</v>
+      </c>
+      <c r="G24" s="30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="H24" s="11"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
@@ -794,15 +1006,14 @@
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B26" s="3">
         <v>241</v>
       </c>
       <c r="C26" s="9"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="17"/>
+      <c r="D26" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="H26" s="11"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
@@ -817,10 +1028,7 @@
         <v>242</v>
       </c>
       <c r="C27" s="9"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="17"/>
+      <c r="D27" s="5"/>
       <c r="H27" s="11"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
@@ -835,10 +1043,13 @@
         <v>255</v>
       </c>
       <c r="C28" s="9"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="17"/>
+      <c r="D28" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="21">
+        <v>6</v>
+      </c>
+      <c r="F28" s="22"/>
       <c r="H28" s="11"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
@@ -853,10 +1064,13 @@
         <v>262</v>
       </c>
       <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="D29" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="27">
+        <f>(B32-B13)/E28</f>
+        <v>45.666666666666664</v>
+      </c>
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
@@ -871,10 +1085,8 @@
         <v>276</v>
       </c>
       <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
@@ -884,15 +1096,23 @@
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
         <v>279</v>
       </c>
       <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
+      <c r="D31" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
@@ -907,10 +1127,21 @@
         <v>282</v>
       </c>
       <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
+      <c r="D32" s="30">
+        <v>8</v>
+      </c>
+      <c r="E32" s="30">
+        <f>D32+E29</f>
+        <v>53.666666666666664</v>
+      </c>
+      <c r="F32" s="23">
+        <f>COUNTIFS($B$13:$B$32,"&gt;="&amp;D32,$B$13:$B$32,"&lt;="&amp;E32)</f>
+        <v>4</v>
+      </c>
+      <c r="G32" s="24">
+        <f>F32/COUNT($B$13:$B$32)</f>
+        <v>0.2</v>
+      </c>
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
@@ -922,10 +1153,22 @@
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
+      <c r="D33" s="30">
+        <f>E32</f>
+        <v>53.666666666666664</v>
+      </c>
+      <c r="E33" s="30">
+        <f>D33+E29</f>
+        <v>99.333333333333329</v>
+      </c>
+      <c r="F33" s="23">
+        <f t="shared" ref="F33:F37" si="2">COUNTIFS($B$13:$B$32,"&gt;="&amp;D33,$B$13:$B$32,"&lt;="&amp;E33)</f>
+        <v>2</v>
+      </c>
+      <c r="G33" s="24">
+        <f t="shared" ref="G33:G38" si="3">F33/COUNT($B$13:$B$32)</f>
+        <v>0.1</v>
+      </c>
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
@@ -937,10 +1180,22 @@
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
+      <c r="D34" s="30">
+        <f>E33</f>
+        <v>99.333333333333329</v>
+      </c>
+      <c r="E34" s="30">
+        <f>D34+E29</f>
+        <v>145</v>
+      </c>
+      <c r="F34" s="23">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G34" s="24">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
@@ -952,10 +1207,22 @@
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
+      <c r="D35" s="30">
+        <f>E34</f>
+        <v>145</v>
+      </c>
+      <c r="E35" s="30">
+        <f>D35+E29</f>
+        <v>190.66666666666666</v>
+      </c>
+      <c r="F35" s="23">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G35" s="24">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
@@ -967,10 +1234,22 @@
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
+      <c r="D36" s="30">
+        <f>E35</f>
+        <v>190.66666666666666</v>
+      </c>
+      <c r="E36" s="30">
+        <f>D36+E29</f>
+        <v>236.33333333333331</v>
+      </c>
+      <c r="F36" s="23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G36" s="24">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
@@ -982,10 +1261,22 @@
     </row>
     <row r="37" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
+      <c r="D37" s="31">
+        <f>E36</f>
+        <v>236.33333333333331</v>
+      </c>
+      <c r="E37" s="31">
+        <f>D37+E29</f>
+        <v>282</v>
+      </c>
+      <c r="F37" s="32">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G37" s="33">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
@@ -998,8 +1289,14 @@
     <row r="38" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D38" s="9"/>
       <c r="E38" s="18"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
+      <c r="F38" s="23">
+        <f>SUM(F32:F37)</f>
+        <v>20</v>
+      </c>
+      <c r="G38" s="30">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
@@ -1122,7 +1419,7 @@
       <c r="O46" s="9"/>
     </row>
   </sheetData>
-  <sortState ref="B13:B32">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B13:B32">
     <sortCondition ref="B13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>